<commit_message>
Mise à jour du tableau E5
</commit_message>
<xml_diff>
--- a/images/E4 - Tableau de synthèse.xlsx
+++ b/images/E4 - Tableau de synthèse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpechartreux-my.sharepoint.com/personal/m_bezettorres_eleve_leschartreux_net/Documents/! SISR/STAGE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpechartreux-my.sharepoint.com/personal/m_bezettorres_eleve_leschartreux_net/Documents/! SISR/Portfolio/Personnal-portfolio/Portfolio/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{65AAFE24-D32F-4309-9CEF-03FB3203825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB2F7AC7-93C2-4D96-800B-91CE37D7CD8C}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{65AAFE24-D32F-4309-9CEF-03FB3203825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CDC4DAA-06CA-4599-9BBB-647A5729A088}"/>
   <bookViews>
-    <workbookView xWindow="13545" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
 </t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
@@ -131,12 +128,6 @@
     <t>Centre de formation : Institution les Chartreux</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio : bezettorres.live</t>
-  </si>
-  <si>
-    <t>SESSION 2024</t>
-  </si>
-  <si>
     <t>Traiter des demandes concernant les services réseau et système via GLPI, gestionnaire de parc informatique</t>
   </si>
   <si>
@@ -162,6 +153,15 @@
   </si>
   <si>
     <t>Support et formation des utilisateurs sur les nouveaux outils et systèmes déployés</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : bezettorres.me</t>
+  </si>
+  <si>
+    <t>SESSION 2025</t>
+  </si>
+  <si>
+    <t>Cette réalisation a pour but de déployer un WIFI invité pour une entreprise fictive.</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -707,15 +707,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -748,42 +778,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1095,8 +1089,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1118,7 +1112,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="H1" s="23"/>
     </row>
@@ -1135,32 +1129,32 @@
       <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="41" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="31"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
+      <c r="A4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="21" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="18" t="s">
@@ -1168,22 +1162,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="A5" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1206,8 +1200,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="19" t="s">
         <v>14</v>
       </c>
@@ -1263,16 +1257,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1311,12 +1305,12 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="44"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -1358,17 +1352,15 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="44"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="H10" s="15"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1406,13 +1398,15 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="B11" s="8"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="15"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -1766,16 +1760,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="A19" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1814,11 +1808,11 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="14"/>
-      <c r="D20" s="44"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
@@ -1861,14 +1855,14 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="44"/>
+        <v>27</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="45"/>
+      <c r="G21" s="14"/>
       <c r="H21" s="15"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -1908,13 +1902,13 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="14"/>
-      <c r="D22" s="45"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="44"/>
+      <c r="F22" s="22"/>
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
       <c r="I22"/>
@@ -1955,13 +1949,13 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="44"/>
+      <c r="F23" s="22"/>
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
       <c r="I23"/>
@@ -2002,14 +1996,14 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="44"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="15"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -2049,14 +2043,14 @@
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="44"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="15"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -2096,14 +2090,14 @@
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="44"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="15"/>
       <c r="I26"/>
       <c r="J26"/>
@@ -2142,16 +2136,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
+      <c r="A27" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2596,11 +2590,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2608,6 +2597,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2624,6 +2618,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F67FAFFF6622EA46A56A0B9F9D3D6381" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b3a53a3eb87022b0bb5d57aedb29600a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="256d7196-e029-48f3-9020-9ca775305906" xmlns:ns3="df0e35dd-c3e7-462f-87b0-0ac0fa0c6328" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c31759d3de9b648bd59bf6cabffaddef" ns2:_="" ns3:_="">
     <xsd:import namespace="256d7196-e029-48f3-9020-9ca775305906"/>
@@ -2840,15 +2843,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8E0CF9-4DA9-461A-9D42-7F5EDB84B399}">
   <ds:schemaRefs>
@@ -2859,6 +2853,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B017DC1C-DD72-4F98-898D-9D6E1CB4C1E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF4C2BB-12AC-4142-A3E9-28B6F5ADC264}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2875,12 +2877,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B017DC1C-DD72-4F98-898D-9D6E1CB4C1E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>